<commit_message>
calculated nuumber of observations by each individual each year
</commit_message>
<xml_diff>
--- a/input/status_intensity_datafield_descriptions.xlsx
+++ b/input/status_intensity_datafield_descriptions.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alina\Documents\git\Tree_Spotters\input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86862557-74BD-4055-A242-3F73E206DE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Status-Intensity Data" sheetId="1" r:id="rId4"/>
+    <sheet name="Status-Intensity Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="197">
   <si>
     <t>Sequence #</t>
   </si>
@@ -611,58 +616,71 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -952,26 +970,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.25" customWidth="true" style="0"/>
-    <col min="2" max="2" width="27.5" customWidth="true" style="0"/>
-    <col min="3" max="3" width="64.38" customWidth="true" style="0"/>
-    <col min="4" max="4" width="31.75" customWidth="true" style="0"/>
+    <col min="1" max="1" width="9.26171875" customWidth="1"/>
+    <col min="2" max="2" width="27.47265625" customWidth="1"/>
+    <col min="3" max="3" width="64.3671875" customWidth="1"/>
+    <col min="4" max="4" width="31.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" customHeight="1" ht="31.5">
+    <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -985,7 +1000,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    <row r="2" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>10</v>
       </c>
@@ -995,9 +1010,8 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2"/>
-    </row>
-    <row r="3" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="3" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>20</v>
       </c>
@@ -1007,9 +1021,8 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3"/>
-    </row>
-    <row r="4" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="4" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>30</v>
       </c>
@@ -1019,9 +1032,8 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4"/>
-    </row>
-    <row r="5" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="5" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>40</v>
       </c>
@@ -1031,9 +1043,8 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5"/>
-    </row>
-    <row r="6" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="6" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>50</v>
       </c>
@@ -1043,9 +1054,8 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6"/>
-    </row>
-    <row r="7" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="7" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>60</v>
       </c>
@@ -1055,9 +1065,8 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7"/>
-    </row>
-    <row r="8" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="8" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>70</v>
       </c>
@@ -1067,9 +1076,8 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D8"/>
-    </row>
-    <row r="9" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="9" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>80</v>
       </c>
@@ -1079,9 +1087,8 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D9"/>
-    </row>
-    <row r="10" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="10" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>90</v>
       </c>
@@ -1091,9 +1098,8 @@
       <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="D10"/>
-    </row>
-    <row r="11" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="11" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>100</v>
       </c>
@@ -1103,9 +1109,8 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D11"/>
-    </row>
-    <row r="12" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="12" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>110</v>
       </c>
@@ -1115,9 +1120,8 @@
       <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="D12"/>
-    </row>
-    <row r="13" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="13" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>120</v>
       </c>
@@ -1127,9 +1131,8 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="D13"/>
-    </row>
-    <row r="14" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="14" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>130</v>
       </c>
@@ -1139,9 +1142,8 @@
       <c r="C14" t="s">
         <v>29</v>
       </c>
-      <c r="D14"/>
-    </row>
-    <row r="15" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="15" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>140</v>
       </c>
@@ -1151,9 +1153,8 @@
       <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="D15"/>
-    </row>
-    <row r="16" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="16" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>150</v>
       </c>
@@ -1163,9 +1164,8 @@
       <c r="C16" t="s">
         <v>33</v>
       </c>
-      <c r="D16"/>
-    </row>
-    <row r="17" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="17" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>160</v>
       </c>
@@ -1175,9 +1175,8 @@
       <c r="C17" t="s">
         <v>35</v>
       </c>
-      <c r="D17"/>
-    </row>
-    <row r="18" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="18" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>170</v>
       </c>
@@ -1187,9 +1186,8 @@
       <c r="C18" t="s">
         <v>37</v>
       </c>
-      <c r="D18"/>
-    </row>
-    <row r="19" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="19" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>180</v>
       </c>
@@ -1199,9 +1197,8 @@
       <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="D19"/>
-    </row>
-    <row r="20" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="20" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>190</v>
       </c>
@@ -1211,9 +1208,8 @@
       <c r="C20" t="s">
         <v>41</v>
       </c>
-      <c r="D20"/>
-    </row>
-    <row r="21" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="21" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>200</v>
       </c>
@@ -1227,7 +1223,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    <row r="22" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>210</v>
       </c>
@@ -1241,7 +1237,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    <row r="23" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>220</v>
       </c>
@@ -1255,7 +1251,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    <row r="24" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>224</v>
       </c>
@@ -1265,9 +1261,8 @@
       <c r="C24" t="s">
         <v>52</v>
       </c>
-      <c r="D24"/>
-    </row>
-    <row r="25" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="25" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>226</v>
       </c>
@@ -1277,9 +1272,8 @@
       <c r="C25" t="s">
         <v>54</v>
       </c>
-      <c r="D25"/>
-    </row>
-    <row r="26" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="26" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>230</v>
       </c>
@@ -1289,9 +1283,8 @@
       <c r="C26" t="s">
         <v>56</v>
       </c>
-      <c r="D26"/>
-    </row>
-    <row r="27" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="27" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>240</v>
       </c>
@@ -1301,9 +1294,8 @@
       <c r="C27" t="s">
         <v>58</v>
       </c>
-      <c r="D27"/>
-    </row>
-    <row r="28" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="28" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>250</v>
       </c>
@@ -1313,9 +1305,8 @@
       <c r="C28" t="s">
         <v>60</v>
       </c>
-      <c r="D28"/>
-    </row>
-    <row r="29" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="29" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>260</v>
       </c>
@@ -1325,9 +1316,8 @@
       <c r="C29" t="s">
         <v>62</v>
       </c>
-      <c r="D29"/>
-    </row>
-    <row r="30" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="30" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>270</v>
       </c>
@@ -1341,7 +1331,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    <row r="31" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>280</v>
       </c>
@@ -1351,9 +1341,8 @@
       <c r="C31" t="s">
         <v>67</v>
       </c>
-      <c r="D31"/>
-    </row>
-    <row r="32" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="32" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>290</v>
       </c>
@@ -1363,9 +1352,8 @@
       <c r="C32" t="s">
         <v>69</v>
       </c>
-      <c r="D32"/>
-    </row>
-    <row r="33" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="33" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>300</v>
       </c>
@@ -1379,7 +1367,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    <row r="34" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>310</v>
       </c>
@@ -1389,9 +1377,8 @@
       <c r="C34" t="s">
         <v>74</v>
       </c>
-      <c r="D34"/>
-    </row>
-    <row r="35" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="35" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>320</v>
       </c>
@@ -1401,9 +1388,8 @@
       <c r="C35" t="s">
         <v>76</v>
       </c>
-      <c r="D35"/>
-    </row>
-    <row r="36" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="36" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>330</v>
       </c>
@@ -1413,9 +1399,8 @@
       <c r="C36" t="s">
         <v>78</v>
       </c>
-      <c r="D36"/>
-    </row>
-    <row r="37" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="37" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>340</v>
       </c>
@@ -1425,9 +1410,8 @@
       <c r="C37" t="s">
         <v>80</v>
       </c>
-      <c r="D37"/>
-    </row>
-    <row r="38" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="38" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>350</v>
       </c>
@@ -1437,9 +1421,8 @@
       <c r="C38" t="s">
         <v>82</v>
       </c>
-      <c r="D38"/>
-    </row>
-    <row r="39" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="39" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>360</v>
       </c>
@@ -1449,9 +1432,8 @@
       <c r="C39" t="s">
         <v>84</v>
       </c>
-      <c r="D39"/>
-    </row>
-    <row r="40" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="40" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>370</v>
       </c>
@@ -1461,23 +1443,22 @@
       <c r="C40" t="s">
         <v>86</v>
       </c>
-      <c r="D40"/>
-    </row>
-    <row r="41" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="41" spans="1:4" ht="99.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>380</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    <row r="42" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>390</v>
       </c>
@@ -1487,9 +1468,8 @@
       <c r="C42" t="s">
         <v>91</v>
       </c>
-      <c r="D42"/>
-    </row>
-    <row r="43" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="43" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>410</v>
       </c>
@@ -1499,9 +1479,8 @@
       <c r="C43" t="s">
         <v>93</v>
       </c>
-      <c r="D43"/>
-    </row>
-    <row r="44" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="44" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>420</v>
       </c>
@@ -1511,9 +1490,8 @@
       <c r="C44" t="s">
         <v>95</v>
       </c>
-      <c r="D44"/>
-    </row>
-    <row r="45" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="45" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>430</v>
       </c>
@@ -1523,9 +1501,8 @@
       <c r="C45" t="s">
         <v>97</v>
       </c>
-      <c r="D45"/>
-    </row>
-    <row r="46" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="46" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>440</v>
       </c>
@@ -1535,9 +1512,8 @@
       <c r="C46" t="s">
         <v>99</v>
       </c>
-      <c r="D46"/>
-    </row>
-    <row r="47" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="47" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>450</v>
       </c>
@@ -1551,7 +1527,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    <row r="48" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>460</v>
       </c>
@@ -1561,9 +1537,8 @@
       <c r="C48" t="s">
         <v>104</v>
       </c>
-      <c r="D48"/>
-    </row>
-    <row r="49" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="49" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>470</v>
       </c>
@@ -1573,9 +1548,8 @@
       <c r="C49" t="s">
         <v>106</v>
       </c>
-      <c r="D49"/>
-    </row>
-    <row r="50" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="50" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>480</v>
       </c>
@@ -1585,9 +1559,8 @@
       <c r="C50" t="s">
         <v>108</v>
       </c>
-      <c r="D50"/>
-    </row>
-    <row r="51" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="51" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>490</v>
       </c>
@@ -1597,9 +1570,8 @@
       <c r="C51" t="s">
         <v>110</v>
       </c>
-      <c r="D51"/>
-    </row>
-    <row r="52" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="52" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>500</v>
       </c>
@@ -1609,9 +1581,8 @@
       <c r="C52" t="s">
         <v>112</v>
       </c>
-      <c r="D52"/>
-    </row>
-    <row r="53" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="53" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <v>510</v>
       </c>
@@ -1621,9 +1592,8 @@
       <c r="C53" t="s">
         <v>114</v>
       </c>
-      <c r="D53"/>
-    </row>
-    <row r="54" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="54" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>520</v>
       </c>
@@ -1633,9 +1603,8 @@
       <c r="C54" t="s">
         <v>116</v>
       </c>
-      <c r="D54"/>
-    </row>
-    <row r="55" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="55" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <v>530</v>
       </c>
@@ -1645,9 +1614,8 @@
       <c r="C55" t="s">
         <v>118</v>
       </c>
-      <c r="D55"/>
-    </row>
-    <row r="56" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="56" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>540</v>
       </c>
@@ -1657,9 +1625,8 @@
       <c r="C56" t="s">
         <v>120</v>
       </c>
-      <c r="D56"/>
-    </row>
-    <row r="57" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="57" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <v>550</v>
       </c>
@@ -1669,9 +1636,8 @@
       <c r="C57" t="s">
         <v>122</v>
       </c>
-      <c r="D57"/>
-    </row>
-    <row r="58" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="58" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>560</v>
       </c>
@@ -1681,9 +1647,8 @@
       <c r="C58" t="s">
         <v>124</v>
       </c>
-      <c r="D58"/>
-    </row>
-    <row r="59" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="59" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <v>570</v>
       </c>
@@ -1693,9 +1658,8 @@
       <c r="C59" t="s">
         <v>126</v>
       </c>
-      <c r="D59"/>
-    </row>
-    <row r="60" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="60" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <v>580</v>
       </c>
@@ -1705,9 +1669,8 @@
       <c r="C60" t="s">
         <v>128</v>
       </c>
-      <c r="D60"/>
-    </row>
-    <row r="61" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="61" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <v>590</v>
       </c>
@@ -1717,9 +1680,8 @@
       <c r="C61" t="s">
         <v>130</v>
       </c>
-      <c r="D61"/>
-    </row>
-    <row r="62" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="62" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <v>600</v>
       </c>
@@ -1729,9 +1691,8 @@
       <c r="C62" t="s">
         <v>132</v>
       </c>
-      <c r="D62"/>
-    </row>
-    <row r="63" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="63" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <v>610</v>
       </c>
@@ -1741,9 +1702,8 @@
       <c r="C63" t="s">
         <v>134</v>
       </c>
-      <c r="D63"/>
-    </row>
-    <row r="64" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="64" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>620</v>
       </c>
@@ -1753,9 +1713,8 @@
       <c r="C64" t="s">
         <v>136</v>
       </c>
-      <c r="D64"/>
-    </row>
-    <row r="65" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="65" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <v>630</v>
       </c>
@@ -1765,9 +1724,8 @@
       <c r="C65" t="s">
         <v>138</v>
       </c>
-      <c r="D65"/>
-    </row>
-    <row r="66" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="66" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <v>640</v>
       </c>
@@ -1777,9 +1735,8 @@
       <c r="C66" t="s">
         <v>140</v>
       </c>
-      <c r="D66"/>
-    </row>
-    <row r="67" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="67" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
         <v>650</v>
       </c>
@@ -1789,9 +1746,8 @@
       <c r="C67" t="s">
         <v>142</v>
       </c>
-      <c r="D67"/>
-    </row>
-    <row r="68" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="68" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <v>660</v>
       </c>
@@ -1801,9 +1757,8 @@
       <c r="C68" t="s">
         <v>144</v>
       </c>
-      <c r="D68"/>
-    </row>
-    <row r="69" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="69" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <v>670</v>
       </c>
@@ -1813,9 +1768,8 @@
       <c r="C69" t="s">
         <v>146</v>
       </c>
-      <c r="D69"/>
-    </row>
-    <row r="70" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="70" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <v>710</v>
       </c>
@@ -1825,9 +1779,8 @@
       <c r="C70" t="s">
         <v>148</v>
       </c>
-      <c r="D70"/>
-    </row>
-    <row r="71" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="71" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
         <v>720</v>
       </c>
@@ -1837,9 +1790,8 @@
       <c r="C71" t="s">
         <v>150</v>
       </c>
-      <c r="D71"/>
-    </row>
-    <row r="72" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="72" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
         <v>730</v>
       </c>
@@ -1849,9 +1801,8 @@
       <c r="C72" t="s">
         <v>152</v>
       </c>
-      <c r="D72"/>
-    </row>
-    <row r="73" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="73" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73">
         <v>740</v>
       </c>
@@ -1861,9 +1812,8 @@
       <c r="C73" t="s">
         <v>154</v>
       </c>
-      <c r="D73"/>
-    </row>
-    <row r="74" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="74" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74">
         <v>750</v>
       </c>
@@ -1873,9 +1823,8 @@
       <c r="C74" t="s">
         <v>156</v>
       </c>
-      <c r="D74"/>
-    </row>
-    <row r="75" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="75" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75">
         <v>760</v>
       </c>
@@ -1885,9 +1834,8 @@
       <c r="C75" t="s">
         <v>158</v>
       </c>
-      <c r="D75"/>
-    </row>
-    <row r="76" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="76" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
         <v>770</v>
       </c>
@@ -1897,9 +1845,8 @@
       <c r="C76" t="s">
         <v>160</v>
       </c>
-      <c r="D76"/>
-    </row>
-    <row r="77" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="77" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77">
         <v>780</v>
       </c>
@@ -1909,9 +1856,8 @@
       <c r="C77" t="s">
         <v>162</v>
       </c>
-      <c r="D77"/>
-    </row>
-    <row r="78" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="78" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78">
         <v>790</v>
       </c>
@@ -1921,9 +1867,8 @@
       <c r="C78" t="s">
         <v>164</v>
       </c>
-      <c r="D78"/>
-    </row>
-    <row r="79" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="79" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79">
         <v>800</v>
       </c>
@@ -1933,9 +1878,8 @@
       <c r="C79" t="s">
         <v>166</v>
       </c>
-      <c r="D79"/>
-    </row>
-    <row r="80" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="80" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80">
         <v>810</v>
       </c>
@@ -1945,9 +1889,8 @@
       <c r="C80" t="s">
         <v>168</v>
       </c>
-      <c r="D80"/>
-    </row>
-    <row r="81" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="81" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81">
         <v>820</v>
       </c>
@@ -1957,9 +1900,8 @@
       <c r="C81" t="s">
         <v>170</v>
       </c>
-      <c r="D81"/>
-    </row>
-    <row r="82" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="82" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82">
         <v>830</v>
       </c>
@@ -1969,9 +1911,8 @@
       <c r="C82" t="s">
         <v>172</v>
       </c>
-      <c r="D82"/>
-    </row>
-    <row r="83" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="83" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83">
         <v>840</v>
       </c>
@@ -1981,9 +1922,8 @@
       <c r="C83" t="s">
         <v>174</v>
       </c>
-      <c r="D83"/>
-    </row>
-    <row r="84" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="84" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84">
         <v>850</v>
       </c>
@@ -1993,9 +1933,8 @@
       <c r="C84" t="s">
         <v>176</v>
       </c>
-      <c r="D84"/>
-    </row>
-    <row r="85" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="85" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85">
         <v>860</v>
       </c>
@@ -2005,9 +1944,8 @@
       <c r="C85" t="s">
         <v>178</v>
       </c>
-      <c r="D85"/>
-    </row>
-    <row r="86" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="86" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86">
         <v>870</v>
       </c>
@@ -2017,9 +1955,8 @@
       <c r="C86" t="s">
         <v>180</v>
       </c>
-      <c r="D86"/>
-    </row>
-    <row r="87" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="87" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87">
         <v>880</v>
       </c>
@@ -2029,9 +1966,8 @@
       <c r="C87" t="s">
         <v>182</v>
       </c>
-      <c r="D87"/>
-    </row>
-    <row r="88" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="88" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88">
         <v>890</v>
       </c>
@@ -2041,9 +1977,8 @@
       <c r="C88" t="s">
         <v>184</v>
       </c>
-      <c r="D88"/>
-    </row>
-    <row r="89" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="89" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89">
         <v>900</v>
       </c>
@@ -2053,9 +1988,8 @@
       <c r="C89" t="s">
         <v>186</v>
       </c>
-      <c r="D89"/>
-    </row>
-    <row r="90" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="90" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90">
         <v>910</v>
       </c>
@@ -2065,9 +1999,8 @@
       <c r="C90" t="s">
         <v>188</v>
       </c>
-      <c r="D90"/>
-    </row>
-    <row r="91" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="91" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91">
         <v>920</v>
       </c>
@@ -2077,9 +2010,8 @@
       <c r="C91" t="s">
         <v>190</v>
       </c>
-      <c r="D91"/>
-    </row>
-    <row r="92" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="92" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92">
         <v>930</v>
       </c>
@@ -2089,9 +2021,8 @@
       <c r="C92" t="s">
         <v>192</v>
       </c>
-      <c r="D92"/>
-    </row>
-    <row r="93" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="93" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93">
         <v>940</v>
       </c>
@@ -2101,9 +2032,8 @@
       <c r="C93" t="s">
         <v>194</v>
       </c>
-      <c r="D93"/>
-    </row>
-    <row r="94" spans="1:4" customHeight="1" ht="31.5" s="0" customFormat="1">
+    </row>
+    <row r="94" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94">
         <v>950</v>
       </c>
@@ -2113,20 +2043,9 @@
       <c r="C94" t="s">
         <v>196</v>
       </c>
-      <c r="D94"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>